<commit_message>
added more test results
</commit_message>
<xml_diff>
--- a/HumanDetectionTests.xlsx
+++ b/HumanDetectionTests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="50">
   <si>
     <t>S.No</t>
   </si>
@@ -97,6 +97,75 @@
   </si>
   <si>
     <t>3,5,0</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>10,10,2</t>
+  </si>
+  <si>
+    <t>2,3,0</t>
+  </si>
+  <si>
+    <t>5,2,0</t>
+  </si>
+  <si>
+    <t>2,8,0</t>
+  </si>
+  <si>
+    <t>5,5,0</t>
+  </si>
+  <si>
+    <t>1,0,0</t>
+  </si>
+  <si>
+    <t>10,0,0</t>
+  </si>
+  <si>
+    <t>8,5,0</t>
+  </si>
+  <si>
+    <t>10,5,0</t>
+  </si>
+  <si>
+    <t>2,0,0</t>
+  </si>
+  <si>
+    <t>12,5,0</t>
+  </si>
+  <si>
+    <t>15,5,0</t>
+  </si>
+  <si>
+    <t>6,0,0</t>
+  </si>
+  <si>
+    <t>6,6,0</t>
+  </si>
+  <si>
+    <t>13,5,0</t>
+  </si>
+  <si>
+    <t>5,10,0</t>
+  </si>
+  <si>
+    <t>0,2,0</t>
+  </si>
+  <si>
+    <t>5,15,0</t>
+  </si>
+  <si>
+    <t>5,17,0</t>
+  </si>
+  <si>
+    <t>5,20,0</t>
+  </si>
+  <si>
+    <t>5,25,0</t>
+  </si>
+  <si>
+    <t>5,21,0</t>
   </si>
 </sst>
 </file>
@@ -437,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I17"/>
+  <dimension ref="A2:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -704,6 +773,9 @@
       <c r="H10">
         <v>6.5850000000000001E-4</v>
       </c>
+      <c r="I10" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
@@ -730,8 +802,14 @@
       <c r="H11">
         <v>6.0489999999999999E-5</v>
       </c>
+      <c r="I11" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>10</v>
+      </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
@@ -753,8 +831,14 @@
       <c r="H12">
         <v>1.5430000000000001E-4</v>
       </c>
+      <c r="I12" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>11</v>
+      </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
@@ -776,8 +860,14 @@
       <c r="H13">
         <v>1.4459999999999999E-4</v>
       </c>
+      <c r="I13" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>12</v>
+      </c>
       <c r="B14" t="s">
         <v>11</v>
       </c>
@@ -799,8 +889,14 @@
       <c r="H14">
         <v>5.7140000000000001E-4</v>
       </c>
+      <c r="I14" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>13</v>
+      </c>
       <c r="B15" t="s">
         <v>11</v>
       </c>
@@ -822,15 +918,646 @@
       <c r="H15">
         <v>8.4349999999999998E-3</v>
       </c>
+      <c r="I15" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>14</v>
+      </c>
       <c r="B16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16">
+        <v>2.2569999999999999E-3</v>
+      </c>
+      <c r="G16">
+        <v>3.3089999999999999E-3</v>
+      </c>
+      <c r="H16">
+        <v>4.6069999999999998E-5</v>
+      </c>
+      <c r="I16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>15</v>
+      </c>
       <c r="B17" t="s">
         <v>11</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17">
+        <v>2.2569999999999999E-3</v>
+      </c>
+      <c r="G17">
+        <v>3.3089999999999999E-3</v>
+      </c>
+      <c r="H17">
+        <v>3.2949999999999999E-4</v>
+      </c>
+      <c r="I17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18">
+        <v>2.2569999999999999E-3</v>
+      </c>
+      <c r="G18">
+        <v>3.3089999999999999E-3</v>
+      </c>
+      <c r="H18">
+        <v>1.643E-5</v>
+      </c>
+      <c r="I18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19">
+        <v>2.2569999999999999E-3</v>
+      </c>
+      <c r="G19">
+        <v>3.3089999999999999E-3</v>
+      </c>
+      <c r="H19">
+        <v>3.3639999999999999E-4</v>
+      </c>
+      <c r="I19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20">
+        <v>2.2569999999999999E-3</v>
+      </c>
+      <c r="G20">
+        <v>3.3089999999999999E-3</v>
+      </c>
+      <c r="H20">
+        <v>6.5979999999999999E-4</v>
+      </c>
+      <c r="I20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21">
+        <v>1.11092E-2</v>
+      </c>
+      <c r="G21">
+        <v>6.3090000000000004E-3</v>
+      </c>
+      <c r="H21">
+        <v>5.9699999999999998E-4</v>
+      </c>
+      <c r="I21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22">
+        <v>1.11092E-2</v>
+      </c>
+      <c r="G22">
+        <v>6.3090000000000004E-3</v>
+      </c>
+      <c r="H22">
+        <v>2.1540000000000001E-3</v>
+      </c>
+      <c r="I22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23">
+        <v>3.0490000000000001E-3</v>
+      </c>
+      <c r="G23">
+        <v>4.1989999999999996E-3</v>
+      </c>
+      <c r="H23">
+        <v>1.462E-4</v>
+      </c>
+      <c r="I23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24">
+        <v>2.6259999999999999E-3</v>
+      </c>
+      <c r="G24">
+        <v>2.039E-3</v>
+      </c>
+      <c r="H24">
+        <v>7.4880000000000001E-5</v>
+      </c>
+      <c r="I24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" t="s">
+        <v>37</v>
+      </c>
+      <c r="F25">
+        <v>2.6259999999999999E-3</v>
+      </c>
+      <c r="G25">
+        <v>2.039E-3</v>
+      </c>
+      <c r="H25">
+        <v>2.0719999999999999E-4</v>
+      </c>
+      <c r="I25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" t="s">
+        <v>37</v>
+      </c>
+      <c r="F26">
+        <v>1.781E-3</v>
+      </c>
+      <c r="G26">
+        <v>1.441E-3</v>
+      </c>
+      <c r="H26">
+        <v>1.209E-4</v>
+      </c>
+      <c r="I26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27" t="s">
+        <v>37</v>
+      </c>
+      <c r="F27">
+        <v>1.098E-3</v>
+      </c>
+      <c r="G27">
+        <v>9.2270000000000004E-4</v>
+      </c>
+      <c r="H27">
+        <v>6.2689999999999998E-5</v>
+      </c>
+      <c r="I27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" t="s">
+        <v>39</v>
+      </c>
+      <c r="E28" t="s">
+        <v>40</v>
+      </c>
+      <c r="F28">
+        <v>1.098E-3</v>
+      </c>
+      <c r="G28">
+        <v>9.2270000000000004E-4</v>
+      </c>
+      <c r="H28">
+        <v>5.9370000000000002E-5</v>
+      </c>
+      <c r="I28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" t="s">
+        <v>39</v>
+      </c>
+      <c r="E29" t="s">
+        <v>41</v>
+      </c>
+      <c r="F29">
+        <v>1.098E-3</v>
+      </c>
+      <c r="G29">
+        <v>9.2270000000000004E-4</v>
+      </c>
+      <c r="H29">
+        <v>3.9979999999999998E-3</v>
+      </c>
+      <c r="I29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" t="s">
+        <v>42</v>
+      </c>
+      <c r="E30" t="s">
+        <v>37</v>
+      </c>
+      <c r="F30">
+        <v>1.4989999999999999E-3</v>
+      </c>
+      <c r="G30">
+        <v>1.2310000000000001E-3</v>
+      </c>
+      <c r="H30">
+        <v>9.5459999999999997E-5</v>
+      </c>
+      <c r="I30" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" t="s">
+        <v>44</v>
+      </c>
+      <c r="F31">
+        <v>1.9689999999999998E-3</v>
+      </c>
+      <c r="G31">
+        <v>7.9550000000000003E-3</v>
+      </c>
+      <c r="H31">
+        <v>1.0790000000000001E-3</v>
+      </c>
+      <c r="I31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" t="s">
+        <v>45</v>
+      </c>
+      <c r="E32" t="s">
+        <v>44</v>
+      </c>
+      <c r="F32">
+        <v>3.5040000000000002E-3</v>
+      </c>
+      <c r="G32">
+        <v>2.7789999999999998E-3</v>
+      </c>
+      <c r="H32">
+        <v>3.9130000000000002E-4</v>
+      </c>
+      <c r="I32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" t="s">
+        <v>46</v>
+      </c>
+      <c r="E33" t="s">
+        <v>44</v>
+      </c>
+      <c r="F33">
+        <v>1.4989999999999999E-3</v>
+      </c>
+      <c r="G33">
+        <v>3.2719999999999998E-4</v>
+      </c>
+      <c r="H33">
+        <v>1.014E-4</v>
+      </c>
+      <c r="I33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" t="s">
+        <v>47</v>
+      </c>
+      <c r="E34" t="s">
+        <v>44</v>
+      </c>
+      <c r="F34">
+        <v>3.1530000000000002E-4</v>
+      </c>
+      <c r="G34">
+        <v>9.0959999999999999E-4</v>
+      </c>
+      <c r="H34">
+        <v>1.1290000000000001E-4</v>
+      </c>
+      <c r="I34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" t="s">
+        <v>48</v>
+      </c>
+      <c r="E35" t="s">
+        <v>44</v>
+      </c>
+      <c r="F35">
+        <v>8.0999999999999996E-4</v>
+      </c>
+      <c r="G35">
+        <v>9.6089999999999999E-4</v>
+      </c>
+      <c r="H35">
+        <v>5.2120000000000002E-5</v>
+      </c>
+      <c r="I35" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" t="s">
+        <v>49</v>
+      </c>
+      <c r="E36" t="s">
+        <v>44</v>
+      </c>
+      <c r="F36">
+        <v>6.3489999999999998E-4</v>
+      </c>
+      <c r="G36">
+        <v>2.14E-4</v>
+      </c>
+      <c r="H36">
+        <v>5.181E-5</v>
+      </c>
+      <c r="I36" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" t="s">
+        <v>49</v>
+      </c>
+      <c r="E37" t="s">
+        <v>31</v>
+      </c>
+      <c r="F37">
+        <v>6.3489999999999998E-4</v>
+      </c>
+      <c r="G37">
+        <v>2.14E-4</v>
+      </c>
+      <c r="H37">
+        <v>1.842E-5</v>
+      </c>
+      <c r="I37" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>